<commit_message>
on local on 08-08-2018 after user upload using excel 2
</commit_message>
<xml_diff>
--- a/public/Download Add Users File.xlsx
+++ b/public/Download Add Users File.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">phone</t>
   </si>
   <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">email/user-id</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
@@ -41,11 +41,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,6 +62,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,8 +111,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -130,12 +140,12 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -145,7 +155,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">

</xml_diff>